<commit_message>
LV Contacts - 30 July 2024
</commit_message>
<xml_diff>
--- a/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
+++ b/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AE10FE-F78C-4ADF-8DF3-137C6B24E0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414BB59-DF8F-4F47-99B1-6EC2739ED16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>CompanyName</t>
   </si>
@@ -39,9 +39,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>ContactTypesValue</t>
-  </si>
-  <si>
     <t>Sample</t>
   </si>
   <si>
@@ -93,75 +90,6 @@
     <t>ActivityCompany</t>
   </si>
   <si>
-    <t>MailingStreet</t>
-  </si>
-  <si>
-    <t>MailingCity</t>
-  </si>
-  <si>
-    <t>MailingState</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Office</t>
-  </si>
-  <si>
-    <t>PhysicalOffice</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>LineOfBusiness</t>
-  </si>
-  <si>
-    <t>ProjectNotifyRole</t>
-  </si>
-  <si>
-    <t>Mentor</t>
-  </si>
-  <si>
-    <t>Street 1</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>FVA</t>
-  </si>
-  <si>
-    <t>AR_FVA_FF</t>
-  </si>
-  <si>
-    <t>Sonika Goyal</t>
-  </si>
-  <si>
     <t>AdminUser</t>
   </si>
   <si>
@@ -169,6 +97,15 @@
   </si>
   <si>
     <t>HR User</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Sample John</t>
+  </si>
+  <si>
+    <t>HRSample Jing</t>
   </si>
 </sst>
 </file>
@@ -496,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,13 +444,13 @@
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,132 +460,68 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G3" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -670,17 +543,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +567,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,18 +576,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>19</v>
+      <c r="A1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -726,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -738,18 +611,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Contacts - Initial - 11 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
+++ b/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414BB59-DF8F-4F47-99B1-6EC2739ED16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D281F5-9EC5-434B-9F7A-3402EB71C789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>CompanyName</t>
   </si>
@@ -106,13 +106,67 @@
   </si>
   <si>
     <t>HRSample Jing</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>MailingStreet</t>
+  </si>
+  <si>
+    <t>MailingCity</t>
+  </si>
+  <si>
+    <t>MailingState</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>LineOfBusiness</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>Street 1</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Associate</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>Street 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +178,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -433,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,9 +508,15 @@
     <col min="5" max="5" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +538,35 @@
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -495,8 +588,35 @@
       <c r="G2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -518,8 +638,36 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Contacts Final - 14 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
+++ b/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D281F5-9EC5-434B-9F7A-3402EB71C789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C3C4A9-5004-4ACD-A33B-13E75EF02BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>CompanyName</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Street 2</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,11 +518,12 @@
     <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,22 +558,25 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -601,22 +611,25 @@
         <v>38</v>
       </c>
       <c r="L2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>41</v>
-      </c>
-      <c r="O2" t="s">
-        <v>42</v>
       </c>
       <c r="P2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -651,18 +664,21 @@
         <v>38</v>
       </c>
       <c r="L3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>40</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>41</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>42</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
29 Jan 2025 - LV Contacts - Final
</commit_message>
<xml_diff>
--- a/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
+++ b/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C3C4A9-5004-4ACD-A33B-13E75EF02BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E063568-64D1-4E96-9A91-ACE78D0880F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>ContactType</t>
   </si>
   <si>
-    <t>ActivityCompany</t>
-  </si>
-  <si>
     <t>AdminUser</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>Houlihan Lokey - NY</t>
   </si>
 </sst>
 </file>
@@ -501,13 +501,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
@@ -540,45 +540,45 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -593,45 +593,45 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>36</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>39</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>40</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" t="s">
-        <v>42</v>
-      </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -646,40 +646,40 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>40</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>41</v>
       </c>
-      <c r="P3" t="s">
-        <v>42</v>
-      </c>
       <c r="Q3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -775,15 +775,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Contacts - Mid - 12 May 2025
</commit_message>
<xml_diff>
--- a/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
+++ b/TestData/T1048_Contact_CreateNewContactRecordTypeHoulihanEmployee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0599FD8F-E99E-4789-95CD-B8E71345315A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCD739A-AEE9-442E-9ADA-DC170DD33893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>CompanyName</t>
   </si>
@@ -63,18 +63,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>HRSample</t>
-  </si>
-  <si>
-    <t>Jing</t>
-  </si>
-  <si>
-    <t>jinghrsample@email.com</t>
-  </si>
-  <si>
-    <t>(123) 754-2210</t>
-  </si>
-  <si>
     <t>UsersType</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>Sample John</t>
   </si>
   <si>
-    <t>HRSample Jing</t>
-  </si>
-  <si>
     <t>MiddleName</t>
   </si>
   <si>
@@ -145,9 +130,6 @@
   </si>
   <si>
     <t>CF</t>
-  </si>
-  <si>
-    <t>Street 2</t>
   </si>
   <si>
     <t>Country</t>
@@ -490,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,45 +513,45 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -584,93 +566,40 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
       <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" t="s">
         <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +617,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -727,7 +656,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -749,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -760,12 +689,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>